<commit_message>
Added file: Błędy zooplus.pl and new tests
Tests: dodawanie produktu do koszyka, wyszukiwanie produktu
</commit_message>
<xml_diff>
--- a/Testowanie zooplus.pl/zooplus.xlsx
+++ b/Testowanie zooplus.pl/zooplus.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a19528353e4f8c7c/Pulpit/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a19528353e4f8c7c/Pulpit/Repo/Testowanie/Testowanie zooplus.pl/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="180" documentId="8_{2BF6EF48-9CD8-45A0-8351-71DE06C70D97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{11F829FA-9382-4D9B-85BD-DCE87E2B803D}"/>
+  <xr:revisionPtr revIDLastSave="223" documentId="8_{2BF6EF48-9CD8-45A0-8351-71DE06C70D97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5C877A88-944D-4782-8F3F-778BCDEC39B4}"/>
   <bookViews>
-    <workbookView xWindow="10200" yWindow="3855" windowWidth="28800" windowHeight="15345" xr2:uid="{6AA2485A-BD93-4652-8BF7-DF2FA6B67BF8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{6AA2485A-BD93-4652-8BF7-DF2FA6B67BF8}"/>
   </bookViews>
   <sheets>
     <sheet name="Konto" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="54">
   <si>
     <t>Opis scenariusza testowego</t>
   </si>
@@ -163,6 +163,42 @@
   </si>
   <si>
     <t>Uzytkownik zostaje wylogowany</t>
+  </si>
+  <si>
+    <t>Dodawanie produktu do koszyka</t>
+  </si>
+  <si>
+    <t>Cosma Original Snackies</t>
+  </si>
+  <si>
+    <t>1. Ze strony głównej dodaj do koszyka  "plusem" dostepny, losowy produkt w ilości 1.</t>
+  </si>
+  <si>
+    <t>2. Przejdź do koszyka i zweryfikuje, czy produkt się w nim znajduje.</t>
+  </si>
+  <si>
+    <t>Produkt znajduję się w koszyku.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wyszukiwanie produktu </t>
+  </si>
+  <si>
+    <t>kangur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wybrany produkt zostaje dodany do koszyka zakupowego. </t>
+  </si>
+  <si>
+    <t>1. Wpisz w pole wyszukiwania słowo kangur</t>
+  </si>
+  <si>
+    <t>2. Zweryfikuj, czy wyświetlone produkty zawierają słowo "kangur" w opisie.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">System zwraca produkty, które mają wyszukiwane słowo w opisie produtu. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wyświetlone produkty mają słowo "kangur" w opisie. </t>
   </si>
 </sst>
 </file>
@@ -456,7 +492,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -476,127 +512,132 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -621,6 +662,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -924,7 +969,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D25" sqref="D25"/>
+      <selection pane="bottomLeft" activeCell="C16" sqref="C16:C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -965,296 +1010,328 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="19"/>
-      <c r="B2" s="9" t="s">
+      <c r="A2" s="47"/>
+      <c r="B2" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="21" t="s">
+      <c r="E2" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="22" t="s">
+      <c r="H2" s="50" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="23"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="13"/>
+      <c r="A3" s="48"/>
+      <c r="B3" s="39"/>
+      <c r="C3" s="45"/>
       <c r="D3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="16"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="24"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="51"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="23"/>
-      <c r="B4" s="10"/>
-      <c r="C4" s="13"/>
+      <c r="A4" s="48"/>
+      <c r="B4" s="39"/>
+      <c r="C4" s="45"/>
       <c r="D4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="E4" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="15"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="24"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="51"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="23"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="13"/>
+      <c r="A5" s="48"/>
+      <c r="B5" s="39"/>
+      <c r="C5" s="45"/>
       <c r="D5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="E5" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="15"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="24"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="39"/>
+      <c r="H5" s="51"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="23"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="13"/>
+      <c r="A6" s="48"/>
+      <c r="B6" s="39"/>
+      <c r="C6" s="45"/>
       <c r="D6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="17"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="24"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="42"/>
+      <c r="G6" s="39"/>
+      <c r="H6" s="51"/>
     </row>
     <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="25"/>
-      <c r="B7" s="26"/>
-      <c r="C7" s="27"/>
-      <c r="D7" s="28" t="s">
+      <c r="A7" s="49"/>
+      <c r="B7" s="40"/>
+      <c r="C7" s="46"/>
+      <c r="D7" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="29" t="s">
+      <c r="E7" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="30"/>
-      <c r="G7" s="26"/>
-      <c r="H7" s="31"/>
+      <c r="F7" s="43"/>
+      <c r="G7" s="40"/>
+      <c r="H7" s="52"/>
     </row>
     <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="32"/>
-      <c r="B8" s="33" t="s">
+      <c r="A8" s="27"/>
+      <c r="B8" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="34" t="s">
+      <c r="C8" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="35" t="s">
+      <c r="D8" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="36"/>
-      <c r="F8" s="18" t="s">
+      <c r="E8" s="16"/>
+      <c r="F8" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="G8" s="18" t="s">
+      <c r="G8" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="H8" s="37" t="s">
+      <c r="H8" s="21" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="38"/>
-      <c r="B9" s="39"/>
-      <c r="C9" s="40"/>
-      <c r="D9" s="41" t="s">
+      <c r="A9" s="28"/>
+      <c r="B9" s="36"/>
+      <c r="C9" s="34"/>
+      <c r="D9" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="51" t="s">
+      <c r="E9" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="F9" s="42"/>
-      <c r="G9" s="42"/>
-      <c r="H9" s="43"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="22"/>
     </row>
     <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="32"/>
-      <c r="B10" s="45" t="s">
+      <c r="A10" s="27"/>
+      <c r="B10" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="47"/>
-      <c r="D10" s="35" t="s">
+      <c r="C10" s="18"/>
+      <c r="D10" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="35"/>
-      <c r="F10" s="45" t="s">
+      <c r="E10" s="16"/>
+      <c r="F10" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="G10" s="45" t="s">
+      <c r="G10" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="H10" s="37" t="s">
+      <c r="H10" s="21" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="48"/>
-      <c r="B11" s="46"/>
-      <c r="C11" s="11"/>
+      <c r="A11" s="37"/>
+      <c r="B11" s="30"/>
+      <c r="C11" s="9"/>
       <c r="D11" s="5" t="s">
         <v>30</v>
       </c>
       <c r="E11" s="5"/>
-      <c r="F11" s="46"/>
-      <c r="G11" s="46"/>
-      <c r="H11" s="49"/>
+      <c r="F11" s="30"/>
+      <c r="G11" s="30"/>
+      <c r="H11" s="32"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="48"/>
-      <c r="B12" s="46"/>
-      <c r="C12" s="11"/>
+      <c r="A12" s="37"/>
+      <c r="B12" s="30"/>
+      <c r="C12" s="9"/>
       <c r="D12" s="5" t="s">
         <v>31</v>
       </c>
       <c r="E12" s="5"/>
-      <c r="F12" s="46"/>
-      <c r="G12" s="46"/>
-      <c r="H12" s="49"/>
+      <c r="F12" s="30"/>
+      <c r="G12" s="30"/>
+      <c r="H12" s="32"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="48"/>
-      <c r="B13" s="46"/>
-      <c r="C13" s="11"/>
+      <c r="A13" s="37"/>
+      <c r="B13" s="30"/>
+      <c r="C13" s="9"/>
       <c r="D13" s="5" t="s">
         <v>32</v>
       </c>
       <c r="E13" s="5"/>
-      <c r="F13" s="46"/>
-      <c r="G13" s="46"/>
-      <c r="H13" s="49"/>
+      <c r="F13" s="30"/>
+      <c r="G13" s="30"/>
+      <c r="H13" s="32"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="48"/>
-      <c r="B14" s="46"/>
+      <c r="A14" s="37"/>
+      <c r="B14" s="30"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E14" s="52" t="s">
+      <c r="E14" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="F14" s="46"/>
-      <c r="G14" s="46"/>
-      <c r="H14" s="49"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="30"/>
+      <c r="H14" s="32"/>
     </row>
     <row r="15" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="38"/>
-      <c r="B15" s="50"/>
-      <c r="C15" s="41"/>
-      <c r="D15" s="41" t="s">
+      <c r="A15" s="28"/>
+      <c r="B15" s="31"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="E15" s="41"/>
-      <c r="F15" s="50"/>
-      <c r="G15" s="50"/>
-      <c r="H15" s="43"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="31"/>
+      <c r="G15" s="31"/>
+      <c r="H15" s="22"/>
     </row>
     <row r="16" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="32"/>
-      <c r="B16" s="18" t="s">
+      <c r="A16" s="27"/>
+      <c r="B16" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="C16" s="44" t="s">
+      <c r="C16" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="D16" s="35" t="s">
+      <c r="D16" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="E16" s="35"/>
-      <c r="F16" s="18" t="s">
+      <c r="E16" s="16"/>
+      <c r="F16" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="G16" s="18" t="s">
+      <c r="G16" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="H16" s="37" t="s">
+      <c r="H16" s="21" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="38"/>
-      <c r="B17" s="42"/>
-      <c r="C17" s="53"/>
-      <c r="D17" s="41" t="s">
+      <c r="A17" s="28"/>
+      <c r="B17" s="26"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="E17" s="41"/>
-      <c r="F17" s="42"/>
-      <c r="G17" s="42"/>
-      <c r="H17" s="43"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="26"/>
+      <c r="G17" s="26"/>
+      <c r="H17" s="22"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="6"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="5"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
+      <c r="A18" s="27"/>
+      <c r="B18" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="E18" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="F18" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="G18" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="H18" s="53" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="28"/>
+      <c r="B19" s="24"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="E19" s="17"/>
+      <c r="F19" s="26"/>
+      <c r="G19" s="24"/>
+      <c r="H19" s="54"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="5"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
+      <c r="A20" s="27"/>
+      <c r="B20" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="C20" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="E20" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="F20" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="G20" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="H20" s="21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="28"/>
+      <c r="B21" s="26"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="E21" s="17"/>
+      <c r="F21" s="26"/>
+      <c r="G21" s="26"/>
+      <c r="H21" s="22"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="5"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
+      <c r="A22" s="6"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
@@ -1297,30 +1374,42 @@
       <c r="H26" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="23">
+  <mergeCells count="35">
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="H20:H21"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="H2:H7"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="H18:H19"/>
+    <mergeCell ref="B2:B7"/>
+    <mergeCell ref="F2:F7"/>
+    <mergeCell ref="G2:G7"/>
+    <mergeCell ref="C2:C7"/>
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="B10:B15"/>
+    <mergeCell ref="A10:A15"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="F10:F15"/>
+    <mergeCell ref="G10:G15"/>
+    <mergeCell ref="H10:H15"/>
     <mergeCell ref="H16:H17"/>
     <mergeCell ref="C16:C17"/>
     <mergeCell ref="B16:B17"/>
     <mergeCell ref="A16:A17"/>
     <mergeCell ref="F16:F17"/>
     <mergeCell ref="G16:G17"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="F10:F15"/>
-    <mergeCell ref="G10:G15"/>
-    <mergeCell ref="H10:H15"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="B10:B15"/>
-    <mergeCell ref="A10:A15"/>
-    <mergeCell ref="B2:B7"/>
-    <mergeCell ref="F2:F7"/>
-    <mergeCell ref="G2:G7"/>
-    <mergeCell ref="C2:C7"/>
-    <mergeCell ref="A2:A7"/>
-    <mergeCell ref="H2:H7"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E9" r:id="rId1" xr:uid="{A9E6E15E-8C46-47FB-8D4D-5EF32666223C}"/>

</xml_diff>